<commit_message>
.gitignore sollte jetzt funktioniere
</commit_message>
<xml_diff>
--- a/Diagramme/GanttDiagramm/Notenplana Gantt.xlsx
+++ b/Diagramme/GanttDiagramm/Notenplana Gantt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
   <si>
     <t xml:space="preserve">Nr</t>
   </si>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">Gebrauchsanleitung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84 Tage g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 Tage ü</t>
   </si>
   <si>
     <t xml:space="preserve">Todo</t>
@@ -195,12 +189,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -216,6 +216,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF8000"/>
         <bgColor rgb="FFFF6600"/>
       </patternFill>
@@ -224,12 +230,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF5983B0"/>
         <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -324,7 +324,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,11 +377,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -393,7 +397,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,15 +409,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,7 +477,7 @@
       <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF5983B0"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -495,7 +499,7 @@
   <dimension ref="A1:BO1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="BA12" activeCellId="0" sqref="AC12:BA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1016,8 +1020,8 @@
       <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -1093,8 +1097,8 @@
       <c r="D6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -1172,13 +1176,13 @@
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
@@ -1249,10 +1253,10 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
@@ -1328,11 +1332,11 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
@@ -1409,15 +1413,15 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="14"/>
       <c r="V10" s="9"/>
       <c r="W10" s="9"/>
       <c r="X10" s="9"/>
@@ -1488,20 +1492,20 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="14"/>
+      <c r="O11" s="16"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="14"/>
       <c r="AC11" s="9"/>
       <c r="AD11" s="9"/>
       <c r="AE11" s="9"/>
@@ -1579,32 +1583,32 @@
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="12"/>
-      <c r="AH12" s="12"/>
-      <c r="AI12" s="12"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="12"/>
-      <c r="AM12" s="12"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
-      <c r="AQ12" s="9"/>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="9"/>
-      <c r="AT12" s="9"/>
-      <c r="AU12" s="9"/>
-      <c r="AV12" s="9"/>
-      <c r="AW12" s="9"/>
-      <c r="AX12" s="9"/>
-      <c r="AY12" s="9"/>
-      <c r="AZ12" s="9"/>
-      <c r="BA12" s="9"/>
-      <c r="BB12" s="13"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+      <c r="AG12" s="17"/>
+      <c r="AH12" s="17"/>
+      <c r="AI12" s="17"/>
+      <c r="AJ12" s="17"/>
+      <c r="AK12" s="17"/>
+      <c r="AL12" s="17"/>
+      <c r="AM12" s="17"/>
+      <c r="AN12" s="15"/>
+      <c r="AO12" s="15"/>
+      <c r="AP12" s="15"/>
+      <c r="AQ12" s="15"/>
+      <c r="AR12" s="15"/>
+      <c r="AS12" s="15"/>
+      <c r="AT12" s="15"/>
+      <c r="AU12" s="15"/>
+      <c r="AV12" s="15"/>
+      <c r="AW12" s="15"/>
+      <c r="AX12" s="15"/>
+      <c r="AY12" s="15"/>
+      <c r="AZ12" s="15"/>
+      <c r="BA12" s="15"/>
+      <c r="BB12" s="14"/>
       <c r="BC12" s="9"/>
       <c r="BD12" s="9"/>
       <c r="BE12" s="9"/>
@@ -1630,7 +1634,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
@@ -1682,10 +1686,10 @@
       <c r="AZ13" s="9"/>
       <c r="BA13" s="9"/>
       <c r="BB13" s="9"/>
-      <c r="BC13" s="9"/>
-      <c r="BD13" s="9"/>
-      <c r="BE13" s="9"/>
-      <c r="BF13" s="13"/>
+      <c r="BC13" s="15"/>
+      <c r="BD13" s="15"/>
+      <c r="BE13" s="15"/>
+      <c r="BF13" s="14"/>
       <c r="BG13" s="9"/>
       <c r="BH13" s="9"/>
       <c r="BI13" s="9"/>
@@ -1762,12 +1766,12 @@
       <c r="BC14" s="9"/>
       <c r="BD14" s="9"/>
       <c r="BE14" s="9"/>
-      <c r="BF14" s="9"/>
-      <c r="BG14" s="9"/>
-      <c r="BH14" s="9"/>
-      <c r="BI14" s="9"/>
+      <c r="BF14" s="15"/>
+      <c r="BG14" s="15"/>
+      <c r="BH14" s="15"/>
+      <c r="BI14" s="15"/>
       <c r="BJ14" s="15"/>
-      <c r="BK14" s="9"/>
+      <c r="BK14" s="14"/>
       <c r="BL14" s="9"/>
       <c r="BM14" s="9"/>
       <c r="BN14" s="9"/>
@@ -1807,14 +1811,14 @@
       <c r="W15" s="9"/>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
-      <c r="AF15" s="9"/>
-      <c r="AG15" s="16"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+      <c r="AF15" s="15"/>
+      <c r="AG15" s="18"/>
       <c r="AH15" s="12"/>
       <c r="AI15" s="12"/>
       <c r="AJ15" s="12"/>
@@ -1914,9 +1918,9 @@
       <c r="BA16" s="9"/>
       <c r="BB16" s="9"/>
       <c r="BC16" s="9"/>
-      <c r="BD16" s="9"/>
-      <c r="BE16" s="17"/>
-      <c r="BF16" s="9"/>
+      <c r="BD16" s="15"/>
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="14"/>
       <c r="BG16" s="9"/>
       <c r="BH16" s="9"/>
       <c r="BI16" s="9"/>
@@ -1988,9 +1992,9 @@
       <c r="AX17" s="9"/>
       <c r="AY17" s="9"/>
       <c r="AZ17" s="9"/>
-      <c r="BA17" s="13"/>
-      <c r="BB17" s="9"/>
-      <c r="BC17" s="9"/>
+      <c r="BA17" s="15"/>
+      <c r="BB17" s="15"/>
+      <c r="BC17" s="14"/>
       <c r="BD17" s="9"/>
       <c r="BE17" s="9"/>
       <c r="BF17" s="9"/>
@@ -2146,9 +2150,7 @@
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="D20" s="10"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2286,9 +2288,7 @@
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="D22" s="10"/>
       <c r="E22" s="11"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -2492,28 +2492,28 @@
       <c r="BO24" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="20"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="0" t="s">
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="20"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>